<commit_message>
fix: incorrect part number
</commit_message>
<xml_diff>
--- a/manufacturing/CYCLONE_BOM.xlsx
+++ b/manufacturing/CYCLONE_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Fan Controller\Project Outputs for Fan Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usfedu-my.sharepoint.com/personal/ahmed1_usf_edu/Documents/Projects/cyclone/manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574D46F9-7505-4D7D-9E92-7112ECA18D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{574D46F9-7505-4D7D-9E92-7112ECA18D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93926915-488D-4951-AEC5-A59DFD522560}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="21000" xr2:uid="{3C871036-473A-4E7D-BAB6-A55037EACBE6}"/>
+    <workbookView xWindow="12110" yWindow="3730" windowWidth="34480" windowHeight="15460" xr2:uid="{3C871036-473A-4E7D-BAB6-A55037EACBE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Fan Controller" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,6 @@
     <t>C318133</t>
   </si>
   <si>
-    <t>MR06X1002FTL</t>
-  </si>
-  <si>
     <t>C103414</t>
   </si>
   <si>
@@ -300,6 +297,9 @@
   </si>
   <si>
     <t>C89040</t>
+  </si>
+  <si>
+    <t>C667640</t>
   </si>
 </sst>
 </file>
@@ -699,7 +699,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -967,7 +967,7 @@
         <v>5</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -987,7 +987,7 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1007,7 +1007,7 @@
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1067,7 +1067,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>